<commit_message>
Upload new PLC program
</commit_message>
<xml_diff>
--- a/rig-spring-preloader.xlsx
+++ b/rig-spring-preloader.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\rig-bxt-spring-preloader\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFA8D2B2-109A-4D76-8399-D2B8FE24DC29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59114AA5-0ABC-4E42-92C9-AC05B914562D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{2D2A40A7-2858-4013-928A-A8FD95D1B3C1}"/>
   </bookViews>
@@ -16,6 +16,9 @@
     <sheet name="without feedback" sheetId="3" r:id="rId1"/>
     <sheet name="with feedback (old)" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'without feedback'!$H$2:$L$31</definedName>
+  </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -440,10 +443,10 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>258418</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>66262</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>482049</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>49697</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2512226" cy="753027"/>
     <xdr:sp macro="" textlink="">
@@ -459,7 +462,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10992679" y="4565375"/>
+          <a:off x="6611179" y="240197"/>
           <a:ext cx="2512226" cy="753027"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -859,10 +862,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC872A-0787-4440-BD19-03A095AB7289}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="G7:Q31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G9" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="U19" sqref="U19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1168,8 +1174,10 @@
     <mergeCell ref="H24:L24"/>
     <mergeCell ref="H28:L28"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <printOptions horizontalCentered="1" verticalCentered="1"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>